<commit_message>
Update BOM, schematic and footprint.
</commit_message>
<xml_diff>
--- a/Hardware/Updated Pluto BOM.xlsx
+++ b/Hardware/Updated Pluto BOM.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NikhilNagarkar\Desktop\pluto-master\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Nikhil\ReTrace\Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5D15488-D35B-4337-BCB9-502557DFD5F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{737B9FAC-CBD7-40BF-976E-9DF498307AEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="52">
   <si>
     <t>References</t>
   </si>
@@ -61,78 +61,27 @@
     <t>ON Semiconductor</t>
   </si>
   <si>
-    <t>BC847BTT1G</t>
-  </si>
-  <si>
     <t>U2</t>
   </si>
   <si>
     <t>LCD-F-91W</t>
   </si>
   <si>
-    <t>C2, C3</t>
-  </si>
-  <si>
-    <t>Capacitor SMD 0402  22pF</t>
-  </si>
-  <si>
     <t>KEMET</t>
   </si>
   <si>
-    <t>C0603C180J5GAC TU.</t>
-  </si>
-  <si>
-    <t>C8, C4, C5, C6, C7</t>
-  </si>
-  <si>
-    <t>Capacitor SMD 0402 100nF</t>
-  </si>
-  <si>
-    <t>C0603C104K5RACTU</t>
-  </si>
-  <si>
     <t>TDK</t>
   </si>
   <si>
-    <t>C1</t>
-  </si>
-  <si>
-    <t>Capacitor SMD 0402 4.7uF</t>
-  </si>
-  <si>
-    <t>C1005X5R0J475K050BC</t>
-  </si>
-  <si>
     <t>U1</t>
   </si>
   <si>
-    <t>R2</t>
-  </si>
-  <si>
-    <t>Resistor SMD 0402 47k</t>
-  </si>
-  <si>
     <t>Yageo</t>
   </si>
   <si>
-    <t>RC0402FR-0747KL</t>
-  </si>
-  <si>
-    <t>R1, R3</t>
-  </si>
-  <si>
-    <t>Resistor SMD 0402 10k</t>
-  </si>
-  <si>
     <t>Vishay</t>
   </si>
   <si>
-    <t>CRCW040210K0FKED</t>
-  </si>
-  <si>
-    <t>Panasonic</t>
-  </si>
-  <si>
     <t>U4</t>
   </si>
   <si>
@@ -161,13 +110,94 @@
   </si>
   <si>
     <t>Pickit 3</t>
+  </si>
+  <si>
+    <t>GCM0335C1H220JA16D</t>
+  </si>
+  <si>
+    <t>Murata</t>
+  </si>
+  <si>
+    <t>Capacitor SMD 0201  22pF</t>
+  </si>
+  <si>
+    <t>C8, C9</t>
+  </si>
+  <si>
+    <t>C1,C2,C3,C4,C5,C6,C10,C11</t>
+  </si>
+  <si>
+    <t>GRM033R6YA104KE14D</t>
+  </si>
+  <si>
+    <t>Capacitor SMD 0201 0.1uF</t>
+  </si>
+  <si>
+    <t>CL05A106MP6NUN8</t>
+  </si>
+  <si>
+    <t>Capacitor SMD 0402 10uF</t>
+  </si>
+  <si>
+    <t>C7</t>
+  </si>
+  <si>
+    <t>RC0201FR-0747KL</t>
+  </si>
+  <si>
+    <t>Resistor SMD 0201 47k</t>
+  </si>
+  <si>
+    <t>RC0201FR-0710KL</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>R4</t>
+  </si>
+  <si>
+    <t>Resistor SMD 0201 10k</t>
+  </si>
+  <si>
+    <t>Resistor SMD 0201 100</t>
+  </si>
+  <si>
+    <t>RC0201FR-07100RL</t>
+  </si>
+  <si>
+    <t>RC0201FR-07200RL</t>
+  </si>
+  <si>
+    <t>Resistor SMD 0201 200</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>R7</t>
+  </si>
+  <si>
+    <t>BC846B,215</t>
+  </si>
+  <si>
+    <t>ABS07-32.768KHZ-T</t>
+  </si>
+  <si>
+    <t>X1</t>
+  </si>
+  <si>
+    <t>Crystal</t>
+  </si>
+  <si>
+    <t>Abracon</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -188,6 +218,12 @@
       <color rgb="FF333333"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -502,10 +538,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -514,12 +550,12 @@
     <col min="2" max="2" width="10.44140625" customWidth="1"/>
     <col min="3" max="3" width="27.88671875" customWidth="1"/>
     <col min="4" max="4" width="18.77734375" customWidth="1"/>
-    <col min="5" max="5" width="20.5546875" customWidth="1"/>
+    <col min="5" max="5" width="22.5546875" customWidth="1"/>
     <col min="6" max="6" width="26.21875" customWidth="1"/>
     <col min="7" max="7" width="19.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -536,13 +572,10 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -555,198 +588,219 @@
       <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="1"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="B3" s="1">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3">
+      <c r="F3">
         <v>1000</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="B4" s="1">
         <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="1">
+        <v>8</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="B7" s="1">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E8" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="1">
+        <v>1</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+      <c r="E9" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="1">
-        <v>5</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="1" t="s">
+      <c r="B12" s="1">
+        <v>1</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" s="1">
+        <v>1</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F14">
+        <v>1539</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="1">
-        <v>1</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" s="1"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" s="1">
-        <v>1</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="F7" s="1"/>
-      <c r="G7">
-        <v>705</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" s="1">
-        <v>1</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F8" s="1"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" s="1">
-        <v>2</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" s="1">
-        <v>1</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="F11" s="1"/>
-      <c r="G11">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C12" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E12" s="4"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C13" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G13">
-        <v>1539</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="G14">
-        <f>SUM(G3:G13)</f>
+      <c r="F15">
+        <f>SUM(F3:F14)</f>
         <v>5244</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>